<commit_message>
Give me a Spot BRO
</commit_message>
<xml_diff>
--- a/Tavares_Caio_SOLO_RUBRIC.xlsx
+++ b/Tavares_Caio_SOLO_RUBRIC.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D699B55A-E349-49BD-B9BC-C3C21748AE73}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{932241B8-8245-47AF-A64F-6683393A15C2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13,6 +13,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="105">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -337,6 +338,9 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>II</t>
   </si>
 </sst>
 </file>
@@ -930,8 +934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1061,7 +1065,7 @@
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92))</f>
@@ -1073,7 +1077,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1126,11 +1130,15 @@
       <c r="D6" s="5">
         <v>4</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="3"/>
+      <c r="E6" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G6" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H6" s="17">
         <f>IF(SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92)  &gt; 20, SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92) - 20,0)</f>
@@ -1210,7 +1218,7 @@
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 20, IF(H10+I4 &gt; 20, 20- I4, H10),0)</f>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 20, IF(I10+J4 &gt; 20, 20- J4, I10),0)</f>
@@ -3261,7 +3269,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Spot Light aint so Spotty
</commit_message>
<xml_diff>
--- a/Tavares_Caio_SOLO_RUBRIC.xlsx
+++ b/Tavares_Caio_SOLO_RUBRIC.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{932241B8-8245-47AF-A64F-6683393A15C2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{286B124D-F76E-4EEE-A746-58F1C83F5530}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13,7 +13,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="105">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -935,7 +934,7 @@
   <dimension ref="A1:L118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1065,7 +1064,7 @@
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92))</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92))</f>
@@ -1077,7 +1076,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1218,7 +1217,7 @@
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 20, IF(H10+I4 &gt; 20, 20- I4, H10),0)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 20, IF(I10+J4 &gt; 20, 20- J4, I10),0)</f>
@@ -1275,11 +1274,15 @@
       <c r="D10" s="5">
         <v>1</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="3"/>
+      <c r="E10" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G10" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="19">
         <f>IF(K4+H4 - 20 &gt; 0, K4+H4 - 20, 0)</f>
@@ -3269,7 +3272,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Create Pixel Shader FIRST or go fk urself.
</commit_message>
<xml_diff>
--- a/Tavares_Caio_SOLO_RUBRIC.xlsx
+++ b/Tavares_Caio_SOLO_RUBRIC.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{286B124D-F76E-4EEE-A746-58F1C83F5530}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3E54463-CC96-4F44-B128-82C67201B0D6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="105">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -934,7 +934,7 @@
   <dimension ref="A1:L118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,7 +1064,7 @@
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92))</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92))</f>
@@ -1076,7 +1076,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1217,7 +1217,7 @@
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 20, IF(H10+I4 &gt; 20, 20- I4, H10),0)</f>
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 20, IF(I10+J4 &gt; 20, 20- J4, I10),0)</f>
@@ -3118,7 +3118,9 @@
       <c r="C91" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D91" s="3"/>
+      <c r="D91" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="E91" s="3"/>
       <c r="F91" s="5"/>
       <c r="G91" s="5"/>
@@ -3138,7 +3140,9 @@
       <c r="C92" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D92" s="3"/>
+      <c r="D92" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="E92" s="3"/>
       <c r="F92" s="5"/>
       <c r="G92" s="5"/>
@@ -3272,7 +3276,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Is memory getting overwritten still?
</commit_message>
<xml_diff>
--- a/Tavares_Caio_SOLO_RUBRIC.xlsx
+++ b/Tavares_Caio_SOLO_RUBRIC.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3E54463-CC96-4F44-B128-82C67201B0D6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{322D614C-323D-4C02-A09C-8BE7DF86775C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -934,7 +934,7 @@
   <dimension ref="A1:L118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3276,7 +3276,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
office is coming together
</commit_message>
<xml_diff>
--- a/Tavares_Caio_SOLO_RUBRIC.xlsx
+++ b/Tavares_Caio_SOLO_RUBRIC.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18BD487E-D68F-44F0-B04D-478D38C2FAC6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB1B3806-117E-499D-ACDA-93DCA2929336}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="106">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -936,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1071,7 +1071,7 @@
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92))</f>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
@@ -1079,7 +1079,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1208,11 +1208,15 @@
       <c r="D8" s="5">
         <v>1</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="3"/>
+      <c r="E8" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G8" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" s="18">
         <f>H4+IF(H4 &lt; 20, IF(K4+H4 &gt; 20, 20- H4, K4),0)</f>
@@ -1224,7 +1228,7 @@
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 20, IF(I10+J4 &gt; 20, 20- J4, I10),0)</f>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1415,7 +1419,9 @@
       <c r="D15" s="5">
         <v>2</v>
       </c>
-      <c r="E15" s="2"/>
+      <c r="E15" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="F15" s="3"/>
       <c r="G15" s="16">
         <f t="shared" si="0"/>
@@ -2613,11 +2619,15 @@
       <c r="D67" s="5">
         <v>4</v>
       </c>
-      <c r="E67" s="2"/>
-      <c r="F67" s="3"/>
+      <c r="E67" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G67" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H67" s="5"/>
       <c r="I67" s="5"/>
@@ -3283,7 +3293,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
2 Cameras Tab to Switch + Shitty look_at feature
</commit_message>
<xml_diff>
--- a/Tavares_Caio_SOLO_RUBRIC.xlsx
+++ b/Tavares_Caio_SOLO_RUBRIC.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB1B3806-117E-499D-ACDA-93DCA2929336}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B2FFB54-87F9-4467-8147-E4A238CDC62A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="106">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -936,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="F72" sqref="F72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1071,7 +1071,7 @@
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92))</f>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
@@ -1079,7 +1079,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>45</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1228,7 +1228,7 @@
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 20, IF(I10+J4 &gt; 20, 20- J4, I10),0)</f>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1936,11 +1936,15 @@
       <c r="D38" s="5">
         <v>1</v>
       </c>
-      <c r="E38" s="2"/>
-      <c r="F38" s="3"/>
+      <c r="E38" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G38" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
@@ -2565,7 +2569,9 @@
       <c r="D65" s="5">
         <v>1</v>
       </c>
-      <c r="E65" s="2"/>
+      <c r="E65" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="F65" s="3"/>
       <c r="G65" s="16">
         <f t="shared" si="0"/>
@@ -2950,11 +2956,15 @@
       <c r="D82" s="5">
         <v>3</v>
       </c>
-      <c r="E82" s="2"/>
-      <c r="F82" s="3"/>
+      <c r="E82" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F82" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G82" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H82" s="5"/>
       <c r="I82" s="5"/>
@@ -3138,7 +3148,9 @@
       <c r="D91" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="E91" s="3"/>
+      <c r="E91" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="F91" s="5"/>
       <c r="G91" s="5"/>
       <c r="H91" s="5"/>
@@ -3160,7 +3172,9 @@
       <c r="D92" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="E92" s="3"/>
+      <c r="E92" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="F92" s="5"/>
       <c r="G92" s="5"/>
       <c r="H92" s="5"/>
@@ -3293,7 +3307,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Specular is working. Thanks Clark
</commit_message>
<xml_diff>
--- a/Tavares_Caio_SOLO_RUBRIC.xlsx
+++ b/Tavares_Caio_SOLO_RUBRIC.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B2FFB54-87F9-4467-8147-E4A238CDC62A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F07BF92-8CB7-44E1-98B8-31D790DC0B9E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="106">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -936,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="F72" sqref="F72"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1071,7 +1071,7 @@
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92))</f>
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
@@ -1079,7 +1079,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1228,7 +1228,7 @@
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 20, IF(I10+J4 &gt; 20, 20- J4, I10),0)</f>
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1422,10 +1422,12 @@
       <c r="E15" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F15" s="3"/>
+      <c r="F15" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G15" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
@@ -2572,10 +2574,12 @@
       <c r="E65" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F65" s="3"/>
+      <c r="F65" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G65" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H65" s="5"/>
       <c r="I65" s="5"/>
@@ -3307,7 +3311,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
RTT and GeoShader please wrk.
</commit_message>
<xml_diff>
--- a/Tavares_Caio_SOLO_RUBRIC.xlsx
+++ b/Tavares_Caio_SOLO_RUBRIC.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F07BF92-8CB7-44E1-98B8-31D790DC0B9E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28BA446C-F425-4715-9ADD-61BA3467A94B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -936,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3311,7 +3311,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>